<commit_message>
Genera Archivo de calibracion Gasific correctamente
</commit_message>
<xml_diff>
--- a/calibration/200828_Campagna_FONDO_neutrones_EFIR_Samples_test.xlsx
+++ b/calibration/200828_Campagna_FONDO_neutrones_EFIR_Samples_test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="188">
   <si>
     <t>Este documento se exportó de Numbers. Cada tabla se convirtió en una hoja de cálculo de Excel. Los demás objetos de las hojas de Numbers se colocaron en distintas hojas de cálculo. Recuerda que el cálculo de fórmulas puede ser diferente en Excel.</t>
   </si>
@@ -267,76 +267,88 @@
     <t>Acc8 Range</t>
   </si>
   <si>
+    <t>ch1_12cm_fast</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>ch2_6cm_epi</t>
+  </si>
+  <si>
+    <t>Force by 0</t>
+  </si>
+  <si>
+    <t>ch3_pb_HE</t>
+  </si>
+  <si>
+    <t>ch4_naked_th</t>
+  </si>
+  <si>
+    <t>Cal_Sis3316_125_0xCC</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>Hard Source</t>
+  </si>
+  <si>
+    <t>Par Source</t>
+  </si>
+  <si>
+    <t>Range Min</t>
+  </si>
+  <si>
+    <t>Range Max</t>
+  </si>
+  <si>
+    <t>Bins</t>
+  </si>
+  <si>
+    <t>Cal Factor</t>
+  </si>
+  <si>
+    <t>Cal Offset</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Make Hist</t>
+  </si>
+  <si>
+    <t>Norte_Poly_12_CAL</t>
+  </si>
+  <si>
+    <t>CalSpec</t>
+  </si>
+  <si>
     <t>Norte_Poly_12</t>
   </si>
   <si>
-    <t>+</t>
+    <t>EFIR</t>
+  </si>
+  <si>
+    <t>Energy keV</t>
+  </si>
+  <si>
+    <t>NorEste_Poly_10_CAL</t>
   </si>
   <si>
     <t>NorEste_Poly_10</t>
   </si>
   <si>
-    <t>Force by 0</t>
+    <t>Este_BHDPE_20_CAL</t>
   </si>
   <si>
     <t>Este_BHDPE_20</t>
   </si>
   <si>
+    <t>Sur_Este_919_CAL</t>
+  </si>
+  <si>
     <t>Sur_Este_919</t>
-  </si>
-  <si>
-    <t>Cal_Sis3316_125_0xCC</t>
-  </si>
-  <si>
-    <t>Calibration</t>
-  </si>
-  <si>
-    <t>Hard Source</t>
-  </si>
-  <si>
-    <t>Par Source</t>
-  </si>
-  <si>
-    <t>Range Min</t>
-  </si>
-  <si>
-    <t>Range Max</t>
-  </si>
-  <si>
-    <t>Bins</t>
-  </si>
-  <si>
-    <t>Cal Factor</t>
-  </si>
-  <si>
-    <t>Cal Offset</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Make Hist</t>
-  </si>
-  <si>
-    <t>Norte_Poly_12_CAL</t>
-  </si>
-  <si>
-    <t>CalSpec</t>
-  </si>
-  <si>
-    <t>EFIR</t>
-  </si>
-  <si>
-    <t>Energy keV</t>
-  </si>
-  <si>
-    <t>NorEste_Poly_10_CAL</t>
-  </si>
-  <si>
-    <t>Este_BHDPE_20_CAL</t>
-  </si>
-  <si>
-    <t>Sur_Este_919_CAL</t>
   </si>
   <si>
     <t>Condition</t>
@@ -2065,7 +2077,7 @@
     </row>
     <row r="15">
       <c r="B15" t="s" s="3">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2076,12 +2088,12 @@
         <v>5</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="3">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2092,7 +2104,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3981,10 +3993,10 @@
         <v>101</v>
       </c>
       <c r="D3" t="s" s="13">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s" s="13">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F3" s="14">
         <v>0</v>
@@ -4002,7 +4014,7 @@
         <v>-23.2288563303214</v>
       </c>
       <c r="K3" t="s" s="13">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L3" s="14">
         <v>1</v>
@@ -4011,16 +4023,16 @@
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" t="s" s="27">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s" s="27">
         <v>101</v>
       </c>
       <c r="D4" t="s" s="27">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s" s="27">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F4" s="26">
         <v>0</v>
@@ -4038,7 +4050,7 @@
         <v>-11.8459448034301</v>
       </c>
       <c r="K4" t="s" s="27">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L4" s="26">
         <v>1</v>
@@ -4047,16 +4059,16 @@
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="12"/>
       <c r="B5" t="s" s="27">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s" s="27">
         <v>101</v>
       </c>
       <c r="D5" t="s" s="27">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s" s="27">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F5" s="26">
         <v>0</v>
@@ -4074,7 +4086,7 @@
         <v>-15.8971007105807</v>
       </c>
       <c r="K5" t="s" s="27">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L5" s="26">
         <v>1</v>
@@ -4083,16 +4095,16 @@
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" t="s" s="27">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s" s="27">
         <v>101</v>
       </c>
       <c r="D6" t="s" s="27">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s" s="27">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F6" s="26">
         <v>0</v>
@@ -4110,7 +4122,7 @@
         <v>-25.632976858345</v>
       </c>
       <c r="K6" t="s" s="27">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L6" s="26">
         <v>1</v>
@@ -4253,7 +4265,7 @@
       <c r="A1" s="12"/>
       <c r="B1" s="8"/>
       <c r="C1" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -4277,28 +4289,28 @@
         <v>8</v>
       </c>
       <c r="D2" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G2" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J2" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K2" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L2" t="s" s="10">
         <v>98</v>
@@ -4307,19 +4319,19 @@
         <v>26</v>
       </c>
       <c r="N2" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O2" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" t="s" s="13">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s" s="13">
         <v>100</v>
@@ -4331,7 +4343,7 @@
         <v>840</v>
       </c>
       <c r="G3" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H3" s="14">
         <v>0</v>
@@ -4346,7 +4358,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L3" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M3" s="14">
         <v>1</v>
@@ -4355,14 +4367,14 @@
         <v>1</v>
       </c>
       <c r="O3" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="8"/>
       <c r="C4" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -4386,28 +4398,28 @@
         <v>8</v>
       </c>
       <c r="D5" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F5" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H5" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I5" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J5" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K5" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L5" t="s" s="10">
         <v>98</v>
@@ -4416,22 +4428,22 @@
         <v>26</v>
       </c>
       <c r="N5" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O5" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" t="s" s="13">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s" s="13">
         <v>124</v>
       </c>
-      <c r="C6" t="s" s="13">
-        <v>120</v>
-      </c>
       <c r="D6" t="s" s="13">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E6" s="14">
         <v>140</v>
@@ -4440,7 +4452,7 @@
         <v>840</v>
       </c>
       <c r="G6" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H6" s="14">
         <v>0</v>
@@ -4455,7 +4467,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L6" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M6" s="14">
         <v>1</v>
@@ -4464,14 +4476,14 @@
         <v>1</v>
       </c>
       <c r="O6" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="8"/>
       <c r="C7" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -4495,28 +4507,28 @@
         <v>8</v>
       </c>
       <c r="D8" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I8" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J8" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K8" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L8" t="s" s="10">
         <v>98</v>
@@ -4525,22 +4537,22 @@
         <v>26</v>
       </c>
       <c r="N8" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O8" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" t="s" s="13">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s" s="13">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E9" s="14">
         <v>140</v>
@@ -4549,7 +4561,7 @@
         <v>840</v>
       </c>
       <c r="G9" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H9" s="14">
         <v>0</v>
@@ -4564,7 +4576,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L9" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M9" s="14">
         <v>1</v>
@@ -4573,14 +4585,14 @@
         <v>1</v>
       </c>
       <c r="O9" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="8"/>
       <c r="C10" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -4604,28 +4616,28 @@
         <v>8</v>
       </c>
       <c r="D11" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G11" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I11" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J11" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K11" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L11" t="s" s="10">
         <v>98</v>
@@ -4634,22 +4646,22 @@
         <v>26</v>
       </c>
       <c r="N11" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O11" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" t="s" s="13">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D12" t="s" s="13">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E12" s="14">
         <v>140</v>
@@ -4658,7 +4670,7 @@
         <v>840</v>
       </c>
       <c r="G12" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H12" s="14">
         <v>0</v>
@@ -4673,7 +4685,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L12" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M12" s="14">
         <v>1</v>
@@ -4682,14 +4694,14 @@
         <v>1</v>
       </c>
       <c r="O12" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="8"/>
       <c r="C13" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -4713,28 +4725,28 @@
         <v>8</v>
       </c>
       <c r="D14" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E14" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F14" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G14" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H14" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I14" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J14" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K14" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L14" t="s" s="10">
         <v>98</v>
@@ -4743,22 +4755,22 @@
         <v>26</v>
       </c>
       <c r="N14" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O14" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" t="s" s="13">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D15" t="s" s="13">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E15" s="14">
         <v>140</v>
@@ -4767,7 +4779,7 @@
         <v>840</v>
       </c>
       <c r="G15" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H15" s="14">
         <v>0</v>
@@ -4782,7 +4794,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L15" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M15" s="14">
         <v>1</v>
@@ -4791,14 +4803,14 @@
         <v>1</v>
       </c>
       <c r="O15" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" s="12"/>
       <c r="B16" s="8"/>
       <c r="C16" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -4822,28 +4834,28 @@
         <v>8</v>
       </c>
       <c r="D17" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F17" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G17" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J17" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K17" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L17" t="s" s="10">
         <v>98</v>
@@ -4852,22 +4864,22 @@
         <v>26</v>
       </c>
       <c r="N17" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O17" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" s="12"/>
       <c r="B18" t="s" s="13">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D18" t="s" s="13">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E18" s="14">
         <v>140</v>
@@ -4876,7 +4888,7 @@
         <v>840</v>
       </c>
       <c r="G18" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H18" s="14">
         <v>0</v>
@@ -4891,7 +4903,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L18" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M18" s="14">
         <v>1</v>
@@ -4900,14 +4912,14 @@
         <v>1</v>
       </c>
       <c r="O18" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" s="12"/>
       <c r="B19" s="8"/>
       <c r="C19" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -4931,28 +4943,28 @@
         <v>8</v>
       </c>
       <c r="D20" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F20" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G20" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H20" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I20" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J20" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K20" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L20" t="s" s="10">
         <v>98</v>
@@ -4961,22 +4973,22 @@
         <v>26</v>
       </c>
       <c r="N20" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O20" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" t="s" s="13">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s" s="13">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E21" s="14">
         <v>140</v>
@@ -4985,7 +4997,7 @@
         <v>840</v>
       </c>
       <c r="G21" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H21" s="14">
         <v>0</v>
@@ -5000,7 +5012,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L21" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M21" s="14">
         <v>1</v>
@@ -5009,14 +5021,14 @@
         <v>1</v>
       </c>
       <c r="O21" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="8"/>
       <c r="C22" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -5040,28 +5052,28 @@
         <v>8</v>
       </c>
       <c r="D23" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E23" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F23" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G23" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H23" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I23" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J23" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K23" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L23" t="s" s="10">
         <v>98</v>
@@ -5070,22 +5082,22 @@
         <v>26</v>
       </c>
       <c r="N23" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O23" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" t="s" s="13">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s" s="13">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E24" s="14">
         <v>140</v>
@@ -5094,7 +5106,7 @@
         <v>840</v>
       </c>
       <c r="G24" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H24" s="14">
         <v>0</v>
@@ -5109,7 +5121,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L24" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M24" s="14">
         <v>1</v>
@@ -5118,14 +5130,14 @@
         <v>1</v>
       </c>
       <c r="O24" t="s" s="13">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="8"/>
       <c r="C25" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -5149,28 +5161,28 @@
         <v>8</v>
       </c>
       <c r="D26" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F26" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G26" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H26" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I26" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J26" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K26" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L26" t="s" s="10">
         <v>98</v>
@@ -5179,19 +5191,19 @@
         <v>26</v>
       </c>
       <c r="N26" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O26" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" ht="13.55" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" t="s" s="13">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s" s="13">
         <v>100</v>
@@ -5203,7 +5215,7 @@
         <v>840</v>
       </c>
       <c r="G27" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H27" s="14">
         <v>0</v>
@@ -5218,7 +5230,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L27" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M27" s="14">
         <v>1</v>
@@ -5227,14 +5239,14 @@
         <v>1</v>
       </c>
       <c r="O27" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" s="12"/>
       <c r="B28" s="8"/>
       <c r="C28" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -5258,28 +5270,28 @@
         <v>8</v>
       </c>
       <c r="D29" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F29" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H29" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I29" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J29" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K29" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L29" t="s" s="10">
         <v>98</v>
@@ -5288,22 +5300,22 @@
         <v>26</v>
       </c>
       <c r="N29" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O29" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" t="s" s="13">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D30" t="s" s="13">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E30" s="14">
         <v>140</v>
@@ -5312,7 +5324,7 @@
         <v>840</v>
       </c>
       <c r="G30" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H30" s="14">
         <v>0</v>
@@ -5327,7 +5339,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L30" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M30" s="14">
         <v>1</v>
@@ -5336,14 +5348,14 @@
         <v>1</v>
       </c>
       <c r="O30" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" ht="13.55" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="8"/>
       <c r="C31" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -5367,28 +5379,28 @@
         <v>8</v>
       </c>
       <c r="D32" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E32" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F32" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G32" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H32" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I32" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J32" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K32" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L32" t="s" s="10">
         <v>98</v>
@@ -5397,22 +5409,22 @@
         <v>26</v>
       </c>
       <c r="N32" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O32" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" s="12"/>
       <c r="B33" t="s" s="13">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D33" t="s" s="13">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E33" s="14">
         <v>140</v>
@@ -5421,7 +5433,7 @@
         <v>840</v>
       </c>
       <c r="G33" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H33" s="14">
         <v>0</v>
@@ -5436,7 +5448,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L33" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M33" s="14">
         <v>1</v>
@@ -5445,14 +5457,14 @@
         <v>1</v>
       </c>
       <c r="O33" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" ht="13.55" customHeight="1">
       <c r="A34" s="12"/>
       <c r="B34" s="8"/>
       <c r="C34" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -5476,28 +5488,28 @@
         <v>8</v>
       </c>
       <c r="D35" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E35" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F35" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G35" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H35" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I35" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J35" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K35" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L35" t="s" s="10">
         <v>98</v>
@@ -5506,22 +5518,22 @@
         <v>26</v>
       </c>
       <c r="N35" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O35" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" ht="13.55" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" t="s" s="13">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D36" t="s" s="13">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E36" s="14">
         <v>140</v>
@@ -5530,7 +5542,7 @@
         <v>840</v>
       </c>
       <c r="G36" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H36" s="14">
         <v>0</v>
@@ -5545,7 +5557,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L36" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M36" s="14">
         <v>1</v>
@@ -5554,14 +5566,14 @@
         <v>1</v>
       </c>
       <c r="O36" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" ht="13.55" customHeight="1">
       <c r="A37" s="12"/>
       <c r="B37" s="8"/>
       <c r="C37" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
@@ -5585,28 +5597,28 @@
         <v>8</v>
       </c>
       <c r="D38" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E38" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F38" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G38" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H38" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I38" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J38" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K38" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L38" t="s" s="10">
         <v>98</v>
@@ -5615,22 +5627,22 @@
         <v>26</v>
       </c>
       <c r="N38" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O38" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" s="12"/>
       <c r="B39" t="s" s="13">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D39" t="s" s="13">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E39" s="14">
         <v>140</v>
@@ -5639,7 +5651,7 @@
         <v>840</v>
       </c>
       <c r="G39" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H39" s="14">
         <v>0</v>
@@ -5654,7 +5666,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L39" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M39" s="14">
         <v>1</v>
@@ -5663,14 +5675,14 @@
         <v>1</v>
       </c>
       <c r="O39" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" ht="13.55" customHeight="1">
       <c r="A40" s="12"/>
       <c r="B40" s="8"/>
       <c r="C40" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -5694,28 +5706,28 @@
         <v>8</v>
       </c>
       <c r="D41" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E41" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F41" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G41" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H41" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I41" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J41" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K41" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L41" t="s" s="10">
         <v>98</v>
@@ -5724,22 +5736,22 @@
         <v>26</v>
       </c>
       <c r="N41" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O41" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" ht="13.55" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" t="s" s="13">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s" s="13">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E42" s="14">
         <v>140</v>
@@ -5748,7 +5760,7 @@
         <v>840</v>
       </c>
       <c r="G42" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H42" s="14">
         <v>0</v>
@@ -5763,7 +5775,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L42" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M42" s="14">
         <v>1</v>
@@ -5772,14 +5784,14 @@
         <v>1</v>
       </c>
       <c r="O42" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" ht="13.55" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="8"/>
       <c r="C43" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -5803,28 +5815,28 @@
         <v>8</v>
       </c>
       <c r="D44" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E44" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F44" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G44" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H44" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I44" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J44" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K44" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L44" t="s" s="10">
         <v>98</v>
@@ -5833,22 +5845,22 @@
         <v>26</v>
       </c>
       <c r="N44" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O44" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" ht="13.55" customHeight="1">
       <c r="A45" s="12"/>
       <c r="B45" t="s" s="13">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D45" t="s" s="13">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E45" s="14">
         <v>140</v>
@@ -5857,7 +5869,7 @@
         <v>840</v>
       </c>
       <c r="G45" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H45" s="14">
         <v>0</v>
@@ -5872,7 +5884,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L45" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M45" s="14">
         <v>1</v>
@@ -5881,14 +5893,14 @@
         <v>1</v>
       </c>
       <c r="O45" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" ht="13.55" customHeight="1">
       <c r="A46" s="12"/>
       <c r="B46" s="8"/>
       <c r="C46" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -5912,28 +5924,28 @@
         <v>8</v>
       </c>
       <c r="D47" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F47" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G47" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H47" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I47" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J47" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K47" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L47" t="s" s="10">
         <v>98</v>
@@ -5942,22 +5954,22 @@
         <v>26</v>
       </c>
       <c r="N47" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O47" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" ht="13.55" customHeight="1">
       <c r="A48" s="12"/>
       <c r="B48" t="s" s="13">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D48" t="s" s="13">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E48" s="14">
         <v>140</v>
@@ -5966,7 +5978,7 @@
         <v>840</v>
       </c>
       <c r="G48" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H48" s="14">
         <v>0</v>
@@ -5981,7 +5993,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L48" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M48" s="14">
         <v>1</v>
@@ -5990,14 +6002,14 @@
         <v>1</v>
       </c>
       <c r="O48" t="s" s="13">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" ht="13.55" customHeight="1">
       <c r="A49" s="12"/>
       <c r="B49" s="8"/>
       <c r="C49" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -6021,28 +6033,28 @@
         <v>8</v>
       </c>
       <c r="D50" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E50" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F50" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G50" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H50" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I50" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J50" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K50" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L50" t="s" s="10">
         <v>98</v>
@@ -6051,19 +6063,19 @@
         <v>26</v>
       </c>
       <c r="N50" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O50" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" ht="13.55" customHeight="1">
       <c r="A51" s="12"/>
       <c r="B51" t="s" s="13">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C51" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s" s="13">
         <v>100</v>
@@ -6075,7 +6087,7 @@
         <v>840</v>
       </c>
       <c r="G51" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H51" s="14">
         <v>0</v>
@@ -6090,7 +6102,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L51" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M51" s="14">
         <v>1</v>
@@ -6099,14 +6111,14 @@
         <v>1</v>
       </c>
       <c r="O51" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" ht="13.55" customHeight="1">
       <c r="A52" s="12"/>
       <c r="B52" s="8"/>
       <c r="C52" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
@@ -6130,28 +6142,28 @@
         <v>8</v>
       </c>
       <c r="D53" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E53" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F53" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G53" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H53" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I53" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J53" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K53" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L53" t="s" s="10">
         <v>98</v>
@@ -6160,22 +6172,22 @@
         <v>26</v>
       </c>
       <c r="N53" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O53" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" ht="13.55" customHeight="1">
       <c r="A54" s="12"/>
       <c r="B54" t="s" s="13">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C54" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D54" t="s" s="13">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E54" s="14">
         <v>140</v>
@@ -6184,7 +6196,7 @@
         <v>840</v>
       </c>
       <c r="G54" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H54" s="14">
         <v>0</v>
@@ -6199,7 +6211,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L54" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M54" s="14">
         <v>1</v>
@@ -6208,14 +6220,14 @@
         <v>1</v>
       </c>
       <c r="O54" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" ht="13.55" customHeight="1">
       <c r="A55" s="12"/>
       <c r="B55" s="8"/>
       <c r="C55" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
@@ -6239,28 +6251,28 @@
         <v>8</v>
       </c>
       <c r="D56" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E56" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F56" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G56" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H56" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I56" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J56" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K56" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L56" t="s" s="10">
         <v>98</v>
@@ -6269,22 +6281,22 @@
         <v>26</v>
       </c>
       <c r="N56" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O56" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" ht="13.55" customHeight="1">
       <c r="A57" s="12"/>
       <c r="B57" t="s" s="13">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C57" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D57" t="s" s="13">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E57" s="14">
         <v>140</v>
@@ -6293,7 +6305,7 @@
         <v>840</v>
       </c>
       <c r="G57" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H57" s="14">
         <v>0</v>
@@ -6308,7 +6320,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L57" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M57" s="14">
         <v>1</v>
@@ -6317,14 +6329,14 @@
         <v>1</v>
       </c>
       <c r="O57" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" ht="13.55" customHeight="1">
       <c r="A58" s="12"/>
       <c r="B58" s="8"/>
       <c r="C58" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
@@ -6348,28 +6360,28 @@
         <v>8</v>
       </c>
       <c r="D59" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E59" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F59" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G59" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H59" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I59" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J59" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K59" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L59" t="s" s="10">
         <v>98</v>
@@ -6378,22 +6390,22 @@
         <v>26</v>
       </c>
       <c r="N59" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O59" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" ht="13.55" customHeight="1">
       <c r="A60" s="12"/>
       <c r="B60" t="s" s="13">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s" s="13">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E60" s="14">
         <v>140</v>
@@ -6402,7 +6414,7 @@
         <v>840</v>
       </c>
       <c r="G60" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H60" s="14">
         <v>0</v>
@@ -6417,7 +6429,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L60" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M60" s="14">
         <v>1</v>
@@ -6426,14 +6438,14 @@
         <v>1</v>
       </c>
       <c r="O60" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" ht="13.55" customHeight="1">
       <c r="A61" s="12"/>
       <c r="B61" s="8"/>
       <c r="C61" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
@@ -6457,28 +6469,28 @@
         <v>8</v>
       </c>
       <c r="D62" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E62" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F62" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G62" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H62" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I62" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J62" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K62" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L62" t="s" s="10">
         <v>98</v>
@@ -6487,22 +6499,22 @@
         <v>26</v>
       </c>
       <c r="N62" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O62" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" ht="13.55" customHeight="1">
       <c r="A63" s="12"/>
       <c r="B63" t="s" s="13">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C63" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D63" t="s" s="13">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E63" s="14">
         <v>140</v>
@@ -6511,7 +6523,7 @@
         <v>840</v>
       </c>
       <c r="G63" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H63" s="14">
         <v>0</v>
@@ -6526,7 +6538,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L63" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M63" s="14">
         <v>1</v>
@@ -6535,14 +6547,14 @@
         <v>1</v>
       </c>
       <c r="O63" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" ht="13.55" customHeight="1">
       <c r="A64" s="12"/>
       <c r="B64" s="8"/>
       <c r="C64" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
@@ -6566,28 +6578,28 @@
         <v>8</v>
       </c>
       <c r="D65" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E65" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F65" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G65" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H65" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I65" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J65" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K65" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L65" t="s" s="10">
         <v>98</v>
@@ -6596,22 +6608,22 @@
         <v>26</v>
       </c>
       <c r="N65" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O65" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" ht="13.55" customHeight="1">
       <c r="A66" s="12"/>
       <c r="B66" t="s" s="13">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C66" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D66" t="s" s="13">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E66" s="14">
         <v>140</v>
@@ -6620,7 +6632,7 @@
         <v>840</v>
       </c>
       <c r="G66" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H66" s="14">
         <v>0</v>
@@ -6635,7 +6647,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L66" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M66" s="14">
         <v>1</v>
@@ -6644,14 +6656,14 @@
         <v>1</v>
       </c>
       <c r="O66" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" ht="13.55" customHeight="1">
       <c r="A67" s="12"/>
       <c r="B67" s="8"/>
       <c r="C67" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
@@ -6675,28 +6687,28 @@
         <v>8</v>
       </c>
       <c r="D68" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E68" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F68" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G68" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H68" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I68" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J68" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K68" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L68" t="s" s="10">
         <v>98</v>
@@ -6705,22 +6717,22 @@
         <v>26</v>
       </c>
       <c r="N68" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O68" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" ht="13.55" customHeight="1">
       <c r="A69" s="12"/>
       <c r="B69" t="s" s="13">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C69" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D69" t="s" s="13">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E69" s="14">
         <v>140</v>
@@ -6729,7 +6741,7 @@
         <v>840</v>
       </c>
       <c r="G69" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H69" s="14">
         <v>0</v>
@@ -6744,7 +6756,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L69" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M69" s="14">
         <v>1</v>
@@ -6753,14 +6765,14 @@
         <v>1</v>
       </c>
       <c r="O69" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" ht="13.55" customHeight="1">
       <c r="A70" s="12"/>
       <c r="B70" s="8"/>
       <c r="C70" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
@@ -6784,28 +6796,28 @@
         <v>8</v>
       </c>
       <c r="D71" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E71" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F71" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G71" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H71" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I71" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J71" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K71" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L71" t="s" s="10">
         <v>98</v>
@@ -6814,22 +6826,22 @@
         <v>26</v>
       </c>
       <c r="N71" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O71" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" ht="13.55" customHeight="1">
       <c r="A72" s="12"/>
       <c r="B72" t="s" s="13">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D72" t="s" s="13">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E72" s="14">
         <v>140</v>
@@ -6838,7 +6850,7 @@
         <v>840</v>
       </c>
       <c r="G72" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H72" s="14">
         <v>0</v>
@@ -6853,7 +6865,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L72" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M72" s="14">
         <v>1</v>
@@ -6862,14 +6874,14 @@
         <v>1</v>
       </c>
       <c r="O72" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" ht="13.55" customHeight="1">
       <c r="A73" s="12"/>
       <c r="B73" s="8"/>
       <c r="C73" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
@@ -6893,28 +6905,28 @@
         <v>8</v>
       </c>
       <c r="D74" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E74" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F74" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G74" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H74" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I74" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J74" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K74" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L74" t="s" s="10">
         <v>98</v>
@@ -6923,22 +6935,22 @@
         <v>26</v>
       </c>
       <c r="N74" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O74" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" ht="13.55" customHeight="1">
       <c r="A75" s="12"/>
       <c r="B75" t="s" s="13">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s" s="13">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E75" s="14">
         <v>800</v>
@@ -6947,7 +6959,7 @@
         <v>3000</v>
       </c>
       <c r="G75" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H75" s="14">
         <v>0</v>
@@ -6962,7 +6974,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L75" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M75" s="14">
         <v>1</v>
@@ -6971,14 +6983,14 @@
         <v>1</v>
       </c>
       <c r="O75" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" ht="13.55" customHeight="1">
       <c r="A76" s="12"/>
       <c r="B76" s="8"/>
       <c r="C76" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
@@ -7002,28 +7014,28 @@
         <v>8</v>
       </c>
       <c r="D77" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E77" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F77" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G77" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H77" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I77" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J77" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K77" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L77" t="s" s="10">
         <v>98</v>
@@ -7032,22 +7044,22 @@
         <v>26</v>
       </c>
       <c r="N77" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O77" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" ht="13.55" customHeight="1">
       <c r="A78" s="12"/>
       <c r="B78" t="s" s="13">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C78" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D78" t="s" s="13">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E78" s="14">
         <v>800</v>
@@ -7056,7 +7068,7 @@
         <v>3000</v>
       </c>
       <c r="G78" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H78" s="14">
         <v>0</v>
@@ -7071,7 +7083,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L78" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M78" s="14">
         <v>1</v>
@@ -7080,14 +7092,14 @@
         <v>1</v>
       </c>
       <c r="O78" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" ht="13.55" customHeight="1">
       <c r="A79" s="12"/>
       <c r="B79" s="8"/>
       <c r="C79" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
@@ -7111,28 +7123,28 @@
         <v>8</v>
       </c>
       <c r="D80" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E80" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F80" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G80" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H80" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I80" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J80" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K80" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L80" t="s" s="10">
         <v>98</v>
@@ -7141,22 +7153,22 @@
         <v>26</v>
       </c>
       <c r="N80" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O80" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" ht="13.55" customHeight="1">
       <c r="A81" s="12"/>
       <c r="B81" t="s" s="13">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C81" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D81" t="s" s="13">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E81" s="14">
         <v>800</v>
@@ -7165,7 +7177,7 @@
         <v>3000</v>
       </c>
       <c r="G81" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H81" s="14">
         <v>0</v>
@@ -7180,7 +7192,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L81" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M81" s="14">
         <v>1</v>
@@ -7189,14 +7201,14 @@
         <v>1</v>
       </c>
       <c r="O81" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" ht="13.55" customHeight="1">
       <c r="A82" s="12"/>
       <c r="B82" s="8"/>
       <c r="C82" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
@@ -7220,28 +7232,28 @@
         <v>8</v>
       </c>
       <c r="D83" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E83" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F83" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G83" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H83" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I83" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J83" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K83" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L83" t="s" s="10">
         <v>98</v>
@@ -7250,22 +7262,22 @@
         <v>26</v>
       </c>
       <c r="N83" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O83" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" ht="13.55" customHeight="1">
       <c r="A84" s="12"/>
       <c r="B84" t="s" s="13">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C84" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D84" t="s" s="13">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E84" s="14">
         <v>800</v>
@@ -7274,7 +7286,7 @@
         <v>3000</v>
       </c>
       <c r="G84" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H84" s="14">
         <v>0</v>
@@ -7289,7 +7301,7 @@
         <v>1.6e-08</v>
       </c>
       <c r="L84" t="s" s="13">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M84" s="14">
         <v>1</v>
@@ -7298,14 +7310,14 @@
         <v>1</v>
       </c>
       <c r="O84" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" ht="13.55" customHeight="1">
       <c r="A85" s="12"/>
       <c r="B85" s="8"/>
       <c r="C85" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
@@ -7329,28 +7341,28 @@
         <v>8</v>
       </c>
       <c r="D86" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E86" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F86" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G86" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H86" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I86" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J86" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K86" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L86" t="s" s="10">
         <v>98</v>
@@ -7359,22 +7371,22 @@
         <v>26</v>
       </c>
       <c r="N86" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O86" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" ht="13.55" customHeight="1">
       <c r="A87" s="12"/>
       <c r="B87" t="s" s="13">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C87" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D87" t="s" s="13">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E87" s="14">
         <v>800</v>
@@ -7383,7 +7395,7 @@
         <v>3000</v>
       </c>
       <c r="G87" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H87" s="14">
         <v>0</v>
@@ -7398,7 +7410,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L87" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M87" s="14">
         <v>1</v>
@@ -7407,14 +7419,14 @@
         <v>1</v>
       </c>
       <c r="O87" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" ht="13.55" customHeight="1">
       <c r="A88" s="12"/>
       <c r="B88" s="8"/>
       <c r="C88" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
@@ -7438,28 +7450,28 @@
         <v>8</v>
       </c>
       <c r="D89" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E89" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F89" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G89" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H89" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I89" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J89" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K89" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L89" t="s" s="10">
         <v>98</v>
@@ -7468,22 +7480,22 @@
         <v>26</v>
       </c>
       <c r="N89" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O89" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" ht="13.55" customHeight="1">
       <c r="A90" s="12"/>
       <c r="B90" t="s" s="13">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C90" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D90" t="s" s="13">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E90" s="14">
         <v>800</v>
@@ -7492,7 +7504,7 @@
         <v>3000</v>
       </c>
       <c r="G90" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H90" s="14">
         <v>0</v>
@@ -7507,7 +7519,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L90" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M90" s="14">
         <v>1</v>
@@ -7516,14 +7528,14 @@
         <v>1</v>
       </c>
       <c r="O90" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="91" ht="13.55" customHeight="1">
       <c r="A91" s="12"/>
       <c r="B91" s="8"/>
       <c r="C91" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
@@ -7547,28 +7559,28 @@
         <v>8</v>
       </c>
       <c r="D92" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E92" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F92" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G92" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H92" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I92" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J92" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K92" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L92" t="s" s="10">
         <v>98</v>
@@ -7577,22 +7589,22 @@
         <v>26</v>
       </c>
       <c r="N92" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O92" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" ht="13.55" customHeight="1">
       <c r="A93" s="12"/>
       <c r="B93" t="s" s="13">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C93" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D93" t="s" s="13">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E93" s="14">
         <v>800</v>
@@ -7601,7 +7613,7 @@
         <v>3000</v>
       </c>
       <c r="G93" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H93" s="14">
         <v>0</v>
@@ -7616,7 +7628,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L93" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M93" s="14">
         <v>1</v>
@@ -7625,14 +7637,14 @@
         <v>1</v>
       </c>
       <c r="O93" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" ht="13.55" customHeight="1">
       <c r="A94" s="12"/>
       <c r="B94" s="8"/>
       <c r="C94" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
@@ -7656,28 +7668,28 @@
         <v>8</v>
       </c>
       <c r="D95" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E95" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F95" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G95" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H95" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I95" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J95" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K95" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L95" t="s" s="10">
         <v>98</v>
@@ -7686,22 +7698,22 @@
         <v>26</v>
       </c>
       <c r="N95" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O95" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="96" ht="13.55" customHeight="1">
       <c r="A96" s="12"/>
       <c r="B96" t="s" s="13">
+        <v>170</v>
+      </c>
+      <c r="C96" t="s" s="13">
+        <v>124</v>
+      </c>
+      <c r="D96" t="s" s="13">
         <v>166</v>
-      </c>
-      <c r="C96" t="s" s="13">
-        <v>120</v>
-      </c>
-      <c r="D96" t="s" s="13">
-        <v>162</v>
       </c>
       <c r="E96" s="14">
         <v>800</v>
@@ -7710,7 +7722,7 @@
         <v>3000</v>
       </c>
       <c r="G96" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H96" s="14">
         <v>0</v>
@@ -7725,7 +7737,7 @@
         <v>2.66666666666667e-10</v>
       </c>
       <c r="L96" t="s" s="13">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M96" s="14">
         <v>1</v>
@@ -7734,14 +7746,14 @@
         <v>1</v>
       </c>
       <c r="O96" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="97" ht="13.55" customHeight="1">
       <c r="A97" s="12"/>
       <c r="B97" s="8"/>
       <c r="C97" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
@@ -7765,28 +7777,28 @@
         <v>8</v>
       </c>
       <c r="D98" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E98" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F98" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G98" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H98" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I98" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J98" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K98" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L98" t="s" s="10">
         <v>98</v>
@@ -7795,22 +7807,22 @@
         <v>26</v>
       </c>
       <c r="N98" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O98" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" ht="13.55" customHeight="1">
       <c r="A99" s="12"/>
       <c r="B99" t="s" s="13">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C99" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D99" t="s" s="13">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E99" s="14">
         <v>800</v>
@@ -7819,7 +7831,7 @@
         <v>3000</v>
       </c>
       <c r="G99" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H99" s="14">
         <v>0</v>
@@ -7834,7 +7846,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L99" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M99" s="14">
         <v>1</v>
@@ -7843,14 +7855,14 @@
         <v>1</v>
       </c>
       <c r="O99" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" ht="13.55" customHeight="1">
       <c r="A100" s="12"/>
       <c r="B100" s="8"/>
       <c r="C100" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
@@ -7874,28 +7886,28 @@
         <v>8</v>
       </c>
       <c r="D101" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E101" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F101" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G101" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H101" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I101" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J101" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K101" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L101" t="s" s="10">
         <v>98</v>
@@ -7904,22 +7916,22 @@
         <v>26</v>
       </c>
       <c r="N101" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O101" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="102" ht="13.55" customHeight="1">
       <c r="A102" s="12"/>
       <c r="B102" t="s" s="13">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C102" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D102" t="s" s="13">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E102" s="14">
         <v>800</v>
@@ -7928,7 +7940,7 @@
         <v>3000</v>
       </c>
       <c r="G102" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H102" s="14">
         <v>0</v>
@@ -7943,7 +7955,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L102" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M102" s="14">
         <v>1</v>
@@ -7952,14 +7964,14 @@
         <v>1</v>
       </c>
       <c r="O102" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" ht="13.55" customHeight="1">
       <c r="A103" s="12"/>
       <c r="B103" s="8"/>
       <c r="C103" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D103" s="8"/>
       <c r="E103" s="8"/>
@@ -7983,28 +7995,28 @@
         <v>8</v>
       </c>
       <c r="D104" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E104" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F104" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G104" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H104" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I104" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J104" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K104" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L104" t="s" s="10">
         <v>98</v>
@@ -8013,22 +8025,22 @@
         <v>26</v>
       </c>
       <c r="N104" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O104" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="105" ht="13.55" customHeight="1">
       <c r="A105" s="12"/>
       <c r="B105" t="s" s="13">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C105" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D105" t="s" s="13">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E105" s="14">
         <v>800</v>
@@ -8037,7 +8049,7 @@
         <v>3000</v>
       </c>
       <c r="G105" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H105" s="14">
         <v>0</v>
@@ -8052,7 +8064,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L105" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M105" s="14">
         <v>1</v>
@@ -8061,14 +8073,14 @@
         <v>1</v>
       </c>
       <c r="O105" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" ht="13.55" customHeight="1">
       <c r="A106" s="12"/>
       <c r="B106" s="8"/>
       <c r="C106" t="s" s="32">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
@@ -8092,28 +8104,28 @@
         <v>8</v>
       </c>
       <c r="D107" t="s" s="10">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E107" t="s" s="10">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F107" t="s" s="10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G107" t="s" s="10">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H107" t="s" s="10">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I107" t="s" s="10">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J107" t="s" s="10">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K107" t="s" s="10">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L107" t="s" s="10">
         <v>98</v>
@@ -8122,22 +8134,22 @@
         <v>26</v>
       </c>
       <c r="N107" t="s" s="10">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O107" t="s" s="11">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="108" ht="13.55" customHeight="1">
       <c r="A108" s="12"/>
       <c r="B108" t="s" s="13">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C108" t="s" s="13">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D108" t="s" s="13">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E108" s="14">
         <v>800</v>
@@ -8146,7 +8158,7 @@
         <v>3000</v>
       </c>
       <c r="G108" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H108" s="14">
         <v>0</v>
@@ -8161,7 +8173,7 @@
         <v>4.44444444444444e-12</v>
       </c>
       <c r="L108" t="s" s="13">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M108" s="14">
         <v>1</v>
@@ -8170,14 +8182,14 @@
         <v>1</v>
       </c>
       <c r="O108" t="s" s="13">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="109" ht="13.55" customHeight="1">
       <c r="A109" s="12"/>
       <c r="B109" s="8"/>
       <c r="C109" t="s" s="32">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
@@ -8201,37 +8213,37 @@
         <v>8</v>
       </c>
       <c r="D110" t="s" s="33">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E110" t="s" s="33">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F110" t="s" s="33">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G110" t="s" s="33">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H110" t="s" s="33">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="I110" t="s" s="33">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="J110" t="s" s="33">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="K110" t="s" s="33">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="L110" t="s" s="33">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M110" t="s" s="33">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="N110" t="s" s="33">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="O110" s="18"/>
     </row>
@@ -8262,7 +8274,7 @@
       <c r="A1" s="12"/>
       <c r="B1" s="8"/>
       <c r="C1" t="s" s="32">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>

</xml_diff>